<commit_message>
Changed order of trim curve measurments
</commit_message>
<xml_diff>
--- a/Post_Flight_Datasheet_07_03_V3.xlsx
+++ b/Post_Flight_Datasheet_07_03_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reini\Documents\LR\3rd year\SVV\Flight dynamics\SVV-Flight-Dynamics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{422EA618-38E7-495F-9C69-4B8D7F4F77AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15084C3-60D2-4150-9DDF-6803D9F0B9F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{EA6B8B9C-D53E-4F58-BDAD-B78DCC837A6B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA6B8B9C-D53E-4F58-BDAD-B78DCC837A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -729,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14EB4C2-7152-42F2-9960-C7947507C77F}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1946,60 +1946,46 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-    </row>
+    <row r="58" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="59" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B59" s="8">
-        <v>2.2222222222222223E-2</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="C59" s="6">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D59" s="6">
-        <v>9210</v>
+        <v>9660</v>
       </c>
       <c r="E59" s="6">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I59" s="6">
-        <v>1</v>
+      <c r="I59" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="J59" s="6">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="K59" s="6">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="L59" s="6">
-        <v>591</v>
-      </c>
-      <c r="M59" s="6" t="s">
-        <v>72</v>
+        <v>622</v>
+      </c>
+      <c r="M59" s="6">
+        <v>-7</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2045,43 +2031,43 @@
     </row>
     <row r="61" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B61" s="8">
-        <v>2.4999999999999998E-2</v>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="C61" s="6">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D61" s="6">
-        <v>9660</v>
+        <v>9210</v>
       </c>
       <c r="E61" s="6">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I61" s="6" t="s">
-        <v>78</v>
+      <c r="I61" s="6">
+        <v>1</v>
       </c>
       <c r="J61" s="6">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="K61" s="6">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="L61" s="6">
-        <v>622</v>
-      </c>
-      <c r="M61" s="6">
-        <v>-7</v>
+        <v>591</v>
+      </c>
+      <c r="M61" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Made file compatible with both ref and true data
</commit_message>
<xml_diff>
--- a/Post_Flight_Datasheet_07_03_V3.xlsx
+++ b/Post_Flight_Datasheet_07_03_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reini\Documents\LR\3rd year\SVV\Flight dynamics\SVV-Flight-Dynamics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15084C3-60D2-4150-9DDF-6803D9F0B9F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEAE6EF-3E08-4EEF-A317-32920C6EC812}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA6B8B9C-D53E-4F58-BDAD-B78DCC837A6B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="69">
   <si>
     <t>Post-Flight Data Sheet AE3202</t>
   </si>
@@ -171,42 +171,6 @@
     <t>[°C]</t>
   </si>
   <si>
-    <t>1,8</t>
-  </si>
-  <si>
-    <t>2,1</t>
-  </si>
-  <si>
-    <t>-1,5</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>-3,8</t>
-  </si>
-  <si>
-    <t>5,3</t>
-  </si>
-  <si>
-    <t>-4,5</t>
-  </si>
-  <si>
-    <t>8,3</t>
-  </si>
-  <si>
-    <t>433,5</t>
-  </si>
-  <si>
-    <t>-6,9</t>
-  </si>
-  <si>
-    <t>10,5</t>
-  </si>
-  <si>
-    <t>-7,2</t>
-  </si>
-  <si>
     <t>* ET = Elapsed Time</t>
   </si>
   <si>
@@ -234,51 +198,6 @@
     <t>[N]</t>
   </si>
   <si>
-    <t>4,6</t>
-  </si>
-  <si>
-    <t>0,5</t>
-  </si>
-  <si>
-    <t>3,7</t>
-  </si>
-  <si>
-    <t>-4,8</t>
-  </si>
-  <si>
-    <t>5,4</t>
-  </si>
-  <si>
-    <t>0,2</t>
-  </si>
-  <si>
-    <t>-5,5</t>
-  </si>
-  <si>
-    <t>6,2</t>
-  </si>
-  <si>
-    <t>-0,2</t>
-  </si>
-  <si>
-    <t>-35,5</t>
-  </si>
-  <si>
-    <t>0,9</t>
-  </si>
-  <si>
-    <t>-2,8</t>
-  </si>
-  <si>
-    <t>1,1</t>
-  </si>
-  <si>
-    <t>53,5</t>
-  </si>
-  <si>
-    <t>-2,2</t>
-  </si>
-  <si>
     <t>Shift in center of gravity</t>
   </si>
   <si>
@@ -289,15 +208,6 @@
   </si>
   <si>
     <t>moved to position:</t>
-  </si>
-  <si>
-    <t>4,7</t>
-  </si>
-  <si>
-    <t>0,4</t>
-  </si>
-  <si>
-    <t>0,1</t>
   </si>
   <si>
     <t>Eigenmotions</t>
@@ -729,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14EB4C2-7152-42F2-9960-C7947507C77F}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1274,8 +1184,8 @@
       <c r="E28" s="6">
         <v>237</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>48</v>
+      <c r="F28" s="6">
+        <v>1.8</v>
       </c>
       <c r="G28" s="6">
         <v>675</v>
@@ -1309,8 +1219,8 @@
       <c r="E29" s="6">
         <v>225</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>49</v>
+      <c r="F29" s="6">
+        <v>2.1</v>
       </c>
       <c r="G29" s="6">
         <v>662</v>
@@ -1321,8 +1231,8 @@
       <c r="I29" s="6">
         <v>416</v>
       </c>
-      <c r="J29" s="6" t="s">
-        <v>50</v>
+      <c r="J29" s="6">
+        <v>-1.5</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -1344,8 +1254,8 @@
       <c r="E30" s="6">
         <v>193</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>51</v>
+      <c r="F30" s="6">
+        <v>3.4</v>
       </c>
       <c r="G30" s="6">
         <v>526</v>
@@ -1356,8 +1266,8 @@
       <c r="I30" s="6">
         <v>445</v>
       </c>
-      <c r="J30" s="6" t="s">
-        <v>52</v>
+      <c r="J30" s="6">
+        <v>-3.8</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -1379,8 +1289,8 @@
       <c r="E31" s="6">
         <v>164</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>53</v>
+      <c r="F31" s="6">
+        <v>5.3</v>
       </c>
       <c r="G31" s="6">
         <v>432</v>
@@ -1391,8 +1301,8 @@
       <c r="I31" s="6">
         <v>483</v>
       </c>
-      <c r="J31" s="6" t="s">
-        <v>54</v>
+      <c r="J31" s="6">
+        <v>-4.5</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -1414,20 +1324,20 @@
       <c r="E32" s="6">
         <v>134</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>55</v>
+      <c r="F32" s="6">
+        <v>8.3000000000000007</v>
       </c>
       <c r="G32" s="6">
         <v>398</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>56</v>
+      <c r="H32" s="6">
+        <v>433.5</v>
       </c>
       <c r="I32" s="6">
         <v>504</v>
       </c>
-      <c r="J32" s="6" t="s">
-        <v>57</v>
+      <c r="J32" s="6">
+        <v>-6.9</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -1449,8 +1359,8 @@
       <c r="E33" s="6">
         <v>120</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>58</v>
+      <c r="F33" s="6">
+        <v>10.5</v>
       </c>
       <c r="G33" s="6">
         <v>436</v>
@@ -1461,8 +1371,8 @@
       <c r="I33" s="6">
         <v>526</v>
       </c>
-      <c r="J33" s="6" t="s">
-        <v>59</v>
+      <c r="J33" s="6">
+        <v>-7.2</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -1489,7 +1399,7 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1519,7 +1429,7 @@
     </row>
     <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1551,7 +1461,7 @@
     </row>
     <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1619,7 +1529,7 @@
     <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="7" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>41</v>
@@ -1787,7 +1697,7 @@
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -1802,7 +1712,7 @@
     </row>
     <row r="52" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1886,13 +1796,13 @@
         <v>35</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>36</v>
@@ -1910,7 +1820,7 @@
     <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="7" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>41</v>
@@ -1931,7 +1841,7 @@
         <v>44</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="J57" s="7" t="s">
         <v>45</v>
@@ -1963,17 +1873,17 @@
       <c r="E59" s="6">
         <v>150</v>
       </c>
-      <c r="F59" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I59" s="6" t="s">
-        <v>78</v>
+      <c r="F59" s="6">
+        <v>6.2</v>
+      </c>
+      <c r="G59" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="H59" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="I59" s="6">
+        <v>-35.5</v>
       </c>
       <c r="J59" s="6">
         <v>446</v>
@@ -2004,14 +1914,14 @@
       <c r="E60" s="6">
         <v>160</v>
       </c>
-      <c r="F60" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>71</v>
+      <c r="F60" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="G60" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="H60" s="6">
+        <v>3.7</v>
       </c>
       <c r="I60" s="6">
         <v>-21</v>
@@ -2025,8 +1935,8 @@
       <c r="L60" s="6">
         <v>607</v>
       </c>
-      <c r="M60" s="6" t="s">
-        <v>75</v>
+      <c r="M60" s="6">
+        <v>-5.5</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2045,14 +1955,14 @@
       <c r="E61" s="6">
         <v>170</v>
       </c>
-      <c r="F61" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>71</v>
+      <c r="F61" s="6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G61" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H61" s="6">
+        <v>3.7</v>
       </c>
       <c r="I61" s="6">
         <v>1</v>
@@ -2066,8 +1976,8 @@
       <c r="L61" s="6">
         <v>591</v>
       </c>
-      <c r="M61" s="6" t="s">
-        <v>72</v>
+      <c r="M61" s="6">
+        <v>-4.8</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2086,14 +1996,14 @@
       <c r="E62" s="6">
         <v>183</v>
       </c>
-      <c r="F62" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>71</v>
+      <c r="F62" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="H62" s="6">
+        <v>3.7</v>
       </c>
       <c r="I62" s="6">
         <v>31</v>
@@ -2107,8 +2017,8 @@
       <c r="L62" s="6">
         <v>659</v>
       </c>
-      <c r="M62" s="6" t="s">
-        <v>80</v>
+      <c r="M62" s="6">
+        <v>-2.8</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2127,17 +2037,17 @@
       <c r="E63" s="6">
         <v>192</v>
       </c>
-      <c r="F63" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I63" s="6" t="s">
-        <v>82</v>
+      <c r="F63" s="6">
+        <v>3.4</v>
+      </c>
+      <c r="G63" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H63" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="I63" s="6">
+        <v>53.5</v>
       </c>
       <c r="J63" s="6">
         <v>470</v>
@@ -2148,8 +2058,8 @@
       <c r="L63" s="6">
         <v>677</v>
       </c>
-      <c r="M63" s="6" t="s">
-        <v>83</v>
+      <c r="M63" s="6">
+        <v>-2.2000000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2190,7 +2100,7 @@
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -2220,7 +2130,7 @@
     </row>
     <row r="68" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2252,7 +2162,7 @@
     </row>
     <row r="70" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2269,13 +2179,13 @@
     </row>
     <row r="71" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="1" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -2321,13 +2231,13 @@
         <v>35</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>36</v>
@@ -2345,7 +2255,7 @@
     <row r="74" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3"/>
       <c r="B74" s="7" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>41</v>
@@ -2366,7 +2276,7 @@
         <v>44</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="J74" s="7" t="s">
         <v>45</v>
@@ -2397,14 +2307,14 @@
       <c r="E75" s="6">
         <v>167</v>
       </c>
-      <c r="F75" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>71</v>
+      <c r="F75" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="G75" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="H75" s="6">
+        <v>3.7</v>
       </c>
       <c r="I75" s="6">
         <v>1</v>
@@ -2418,8 +2328,8 @@
       <c r="L75" s="6">
         <v>694</v>
       </c>
-      <c r="M75" s="6" t="s">
-        <v>72</v>
+      <c r="M75" s="6">
+        <v>-4.8</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2438,14 +2348,14 @@
       <c r="E76" s="6">
         <v>169</v>
       </c>
-      <c r="F76" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H76" s="6" t="s">
-        <v>71</v>
+      <c r="F76" s="6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G76" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H76" s="6">
+        <v>3.7</v>
       </c>
       <c r="I76" s="6">
         <v>-28</v>
@@ -2459,15 +2369,15 @@
       <c r="L76" s="6">
         <v>743</v>
       </c>
-      <c r="M76" s="6" t="s">
-        <v>54</v>
+      <c r="M76" s="6">
+        <v>-4.5</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -2497,7 +2407,7 @@
     </row>
     <row r="79" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -2532,17 +2442,17 @@
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="J81" s="3" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
@@ -2553,17 +2463,17 @@
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="J82" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
@@ -2571,7 +2481,7 @@
     </row>
     <row r="83" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -2579,14 +2489,14 @@
         <v>2.9861111111111113E-2</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="8">
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="I83" s="3"/>
       <c r="J83" s="8">
@@ -2598,7 +2508,7 @@
     </row>
     <row r="84" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -2606,14 +2516,14 @@
         <v>3.2638888888888891E-2</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="8">
         <v>3.4027777777777775E-2</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="I84" s="3"/>
       <c r="J84" s="8">

</xml_diff>

<commit_message>
Made Stat1 & 2 fully compatible for both datasets
</commit_message>
<xml_diff>
--- a/Post_Flight_Datasheet_07_03_V3.xlsx
+++ b/Post_Flight_Datasheet_07_03_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reini\Documents\LR\3rd year\SVV\Flight dynamics\SVV-Flight-Dynamics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEAE6EF-3E08-4EEF-A317-32920C6EC812}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A843CA82-1CE8-4487-8DFE-E8A21A370DED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EA6B8B9C-D53E-4F58-BDAD-B78DCC837A6B}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{EA6B8B9C-D53E-4F58-BDAD-B78DCC837A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="72">
   <si>
     <t>Post-Flight Data Sheet AE3202</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>Spiral</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Tps1eng</t>
   </si>
 </sst>
 </file>
@@ -637,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14EB4C2-7152-42F2-9960-C7947507C77F}">
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,8 +1125,12 @@
       <c r="J25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="K25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1149,8 +1162,12 @@
       <c r="J26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="K26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1164,8 +1181,6 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1199,8 +1214,12 @@
       <c r="J28" s="6">
         <v>0</v>
       </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="K28">
+        <v>3106.04</v>
+      </c>
+      <c r="L28">
+        <v>3413.14</v>
+      </c>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1234,8 +1253,12 @@
       <c r="J29" s="6">
         <v>-1.5</v>
       </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="K29">
+        <v>3086.32</v>
+      </c>
+      <c r="L29">
+        <v>3361.08</v>
+      </c>
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1269,8 +1292,12 @@
       <c r="J30" s="6">
         <v>-3.8</v>
       </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="K30">
+        <v>2323.0500000000002</v>
+      </c>
+      <c r="L30">
+        <v>2616.9499999999998</v>
+      </c>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1304,8 +1331,12 @@
       <c r="J31" s="6">
         <v>-4.5</v>
       </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="K31">
+        <v>1811.51</v>
+      </c>
+      <c r="L31">
+        <v>2174.62</v>
+      </c>
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1339,8 +1370,12 @@
       <c r="J32" s="6">
         <v>-6.9</v>
       </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="K32">
+        <v>1714.73</v>
+      </c>
+      <c r="L32">
+        <v>1981.96</v>
+      </c>
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1374,8 +1409,12 @@
       <c r="J33" s="6">
         <v>-7.2</v>
       </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+      <c r="K33">
+        <v>2088.69</v>
+      </c>
+      <c r="L33">
+        <v>2469.9299999999998</v>
+      </c>
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1659,7 +1698,7 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>6</v>
       </c>
@@ -1676,7 +1715,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>7</v>
       </c>
@@ -1693,7 +1732,7 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="1" t="s">
@@ -1710,7 +1749,7 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>52</v>
       </c>
@@ -1727,7 +1766,7 @@
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1742,7 +1781,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>28</v>
       </c>
@@ -1761,7 +1800,7 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1776,7 +1815,7 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>30</v>
       </c>
@@ -1816,8 +1855,17 @@
       <c r="M56" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N56" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="P56" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="7" t="s">
         <v>51</v>
@@ -1855,9 +1903,18 @@
       <c r="M57" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="59" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>3</v>
       </c>
@@ -1897,8 +1954,17 @@
       <c r="M59" s="6">
         <v>-7</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N59">
+        <v>1947.92</v>
+      </c>
+      <c r="O59">
+        <v>2242.0700000000002</v>
+      </c>
+      <c r="P59">
+        <v>1427.77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>2</v>
       </c>
@@ -1938,8 +2004,17 @@
       <c r="M60" s="6">
         <v>-5.5</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N60">
+        <v>1979.8</v>
+      </c>
+      <c r="O60">
+        <v>2278.42</v>
+      </c>
+      <c r="P60">
+        <v>1479.82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>1</v>
       </c>
@@ -1979,8 +2054,17 @@
       <c r="M61" s="6">
         <v>-4.8</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N61">
+        <v>2016.27</v>
+      </c>
+      <c r="O61">
+        <v>2327.48</v>
+      </c>
+      <c r="P61">
+        <v>1537.34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>4</v>
       </c>
@@ -2020,8 +2104,17 @@
       <c r="M62" s="6">
         <v>-2.8</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N62">
+        <v>1931.49</v>
+      </c>
+      <c r="O62">
+        <v>2207.48</v>
+      </c>
+      <c r="P62">
+        <v>1360.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>5</v>
       </c>
@@ -2061,8 +2154,17 @@
       <c r="M63" s="6">
         <v>-2.2000000000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N63">
+        <v>1917.88</v>
+      </c>
+      <c r="O63">
+        <v>2196.9299999999998</v>
+      </c>
+      <c r="P63">
+        <v>1308.32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
update, still not working correct
</commit_message>
<xml_diff>
--- a/Post_Flight_Datasheet_07_03_V3.xlsx
+++ b/Post_Flight_Datasheet_07_03_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxke\Dropbox\Lucht en Ruimtevaart\Third Year Courses\Simulation, Verification and Validation\Python\SVV-Flight-Dynamics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A2754F-B3E3-4721-B4A7-3A5B13B4B40C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C228FD7D-FE5D-452F-BF88-E49E19635934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{EA6B8B9C-D53E-4F58-BDAD-B78DCC837A6B}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14EB4C2-7152-42F2-9960-C7947507C77F}">
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1955,13 +1955,13 @@
         <v>-7</v>
       </c>
       <c r="N59">
-        <v>1947.92</v>
+        <v>2016.27</v>
       </c>
       <c r="O59">
-        <v>2242.0700000000002</v>
+        <v>2327.48</v>
       </c>
       <c r="P59">
-        <v>1427.77</v>
+        <v>1537.34</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2055,13 +2055,13 @@
         <v>-4.8</v>
       </c>
       <c r="N61">
-        <v>2016.27</v>
+        <v>1947.92</v>
       </c>
       <c r="O61">
-        <v>2327.48</v>
+        <v>2242.0700000000002</v>
       </c>
       <c r="P61">
-        <v>1537.34</v>
+        <v>1427.77</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>